<commit_message>
More features shown in examples.
Password protected sheet (pushdown)
Formula rewriting and conditional formatting (advanced server, pushdown and Html->Excel)
</commit_message>
<xml_diff>
--- a/Advanced/TemplaterServer (Java)/resources/templates/Pushdown.xlsx
+++ b/Advanced/TemplaterServer (Java)/resources/templates/Pushdown.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="10995"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="dailyMenu">Sheet1!$B$10:$D$10</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -63,11 +63,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,14 +183,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
     </dxf>
     <dxf>
       <font>
@@ -208,12 +220,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:D6" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:D6" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="B5:D6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Cost"/>
-    <tableColumn id="3" name="Valid on" dataDxfId="0"/>
+    <tableColumn id="3" name="Valid on" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -294,7 +306,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -329,7 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,31 +515,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="23.25">
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="18.75">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -540,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -551,12 +562,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="18.75">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15.75" thickBot="1">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
@@ -567,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15.75" thickTop="1">
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
@@ -578,7 +589,24 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="2:4">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f>B13+C13</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -588,24 +616,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>